<commit_message>
Update: improve comparison label
</commit_message>
<xml_diff>
--- a/file/Book1.xlsx
+++ b/file/Book1.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Ongoing - Dropbox\app-AHP\public\asset\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Ongoing - Dropbox\app-AHP\file\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E9A12B4-B550-4AB0-82CE-DFBC56C4E167}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D40BBD27-FE3C-40B0-9AA0-579478945A13}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15540" windowHeight="10240" xr2:uid="{37971D20-4150-4350-954F-912B86F59D3D}"/>
   </bookViews>
@@ -69,9 +69,6 @@
     <t>test</t>
   </si>
   <si>
-    <t>eetet</t>
-  </si>
-  <si>
     <t>Options</t>
   </si>
   <si>
@@ -90,7 +87,10 @@
     <t>tydy</t>
   </si>
   <si>
-    <t>computer</t>
+    <t>computer computer computer</t>
+  </si>
+  <si>
+    <t>eetet eetet eetet eetet eetet</t>
   </si>
 </sst>
 </file>
@@ -446,17 +446,17 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>15</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>16</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -474,7 +474,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>1</v>
@@ -485,7 +485,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s">
         <v>5</v>
@@ -493,7 +493,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
         <v>2</v>
@@ -522,13 +522,13 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
         <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">

</xml_diff>